<commit_message>
Changes for inclusion of member persona's regression
</commit_message>
<xml_diff>
--- a/Inputs/Announcement-1.xlsx
+++ b/Inputs/Announcement-1.xlsx
@@ -32,10 +32,10 @@
     <t>categoryName</t>
   </si>
   <si>
-    <t>Announcement1-221119</t>
-  </si>
-  <si>
-    <t>Announcement1-221119 Summary</t>
+    <t>Announcement1-230120</t>
+  </si>
+  <si>
+    <t>Announcement1-230120 Summary</t>
   </si>
   <si>
     <t>Africa</t>
@@ -50,10 +50,10 @@
     <t>Planning &amp; Strategy</t>
   </si>
   <si>
-    <t>Announcement2-221119</t>
-  </si>
-  <si>
-    <t>Announcement2-221119 Summary</t>
+    <t>Announcement2-230120</t>
+  </si>
+  <si>
+    <t>Announcement2-230120 Summary</t>
   </si>
   <si>
     <t>Europe</t>
@@ -65,10 +65,10 @@
     <t>Emerging Technologies</t>
   </si>
   <si>
-    <t>Announcement3-221119</t>
-  </si>
-  <si>
-    <t>Announcement3-221119 Summary</t>
+    <t>Announcement3-230120</t>
+  </si>
+  <si>
+    <t>Announcement3-230120 Summary</t>
   </si>
   <si>
     <t>Latin America</t>
@@ -80,10 +80,10 @@
     <t>Staffing &amp; Training</t>
   </si>
   <si>
-    <t>Announcement4-221119</t>
-  </si>
-  <si>
-    <t>Announcement4-221119 Summary</t>
+    <t>Announcement4-230120</t>
+  </si>
+  <si>
+    <t>Announcement4-230120 Summary</t>
   </si>
   <si>
     <t>Middle East</t>
@@ -95,10 +95,10 @@
     <t>Management Technology</t>
   </si>
   <si>
-    <t>Announcement5-221119</t>
-  </si>
-  <si>
-    <t>Announcement5-221119 Summary</t>
+    <t>Announcement5-230120</t>
+  </si>
+  <si>
+    <t>Announcement5-230120 Summary</t>
   </si>
   <si>
     <t>North America</t>
@@ -107,10 +107,10 @@
     <t>Risk &amp; Resiliency</t>
   </si>
   <si>
-    <t>Announcement6-221119</t>
-  </si>
-  <si>
-    <t>Announcement6-221119 Summary</t>
+    <t>Announcement6-230120</t>
+  </si>
+  <si>
+    <t>Announcement6-230120 Summary</t>
   </si>
   <si>
     <t>North Asia</t>
@@ -119,10 +119,10 @@
     <t>New Builds &amp; Equipment</t>
   </si>
   <si>
-    <t>Announcement7-221119</t>
-  </si>
-  <si>
-    <t>Announcement7-221119 Summary</t>
+    <t>Announcement7-230120</t>
+  </si>
+  <si>
+    <t>Announcement7-230120 Summary</t>
   </si>
   <si>
     <t>Russia</t>
@@ -131,10 +131,10 @@
     <t>Distributed Infrastructure</t>
   </si>
   <si>
-    <t>Announcement8-221119</t>
-  </si>
-  <si>
-    <t>Announcement8-221119 Summary</t>
+    <t>Announcement8-230120</t>
+  </si>
+  <si>
+    <t>Announcement8-230120 Summary</t>
   </si>
   <si>
     <t>South Asia</t>

</xml_diff>